<commit_message>
[fully tested code] + rf24 working along with vehicle controller
</commit_message>
<xml_diff>
--- a/Notes/Calibrations.xlsx
+++ b/Notes/Calibrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackxu/JXPlatform/RR2019/RR2019-Hummingbot-Hardware/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492D8591-AF8F-4C49-8D13-B4800F762FA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E9A4B-A5ED-8046-9703-586D9FDC6074}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{1DF121A7-0AAA-1946-92C9-780BA52AB733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Input </t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Delta</t>
+  </si>
+  <si>
+    <t>Resolution:</t>
+  </si>
+  <si>
+    <t>50us</t>
+  </si>
+  <si>
+    <t>5 deg</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -653,11 +662,11 @@
         <v>1684</v>
       </c>
       <c r="C4" s="1">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="D4">
         <f>C4-B4</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -667,11 +676,11 @@
         <v>1500</v>
       </c>
       <c r="J4" s="1">
-        <v>1513</v>
+        <v>1503</v>
       </c>
       <c r="K4">
         <f>J4-I4</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="O4" s="11">
         <v>1800</v>
@@ -691,11 +700,11 @@
         <v>1742</v>
       </c>
       <c r="C5">
-        <v>1763</v>
+        <v>1802</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D10" si="0">C5-B5</f>
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -705,11 +714,11 @@
         <v>1616</v>
       </c>
       <c r="J5">
-        <v>1634</v>
+        <v>1653</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K12" si="1">J5-I5</f>
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="12"/>
@@ -725,11 +734,11 @@
         <v>1788</v>
       </c>
       <c r="C6">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>45</v>
@@ -739,11 +748,11 @@
         <v>1850</v>
       </c>
       <c r="J6">
-        <v>1866</v>
+        <v>1853</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="O6" s="11">
         <v>-90</v>
@@ -812,12 +821,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="O11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:18">
       <c r="K12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="P12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>